<commit_message>
Add question answers, procedure, calcs & graphs to Lab8
</commit_message>
<xml_diff>
--- a/Lab Reports/LabReport10/Lab10SiteData.xlsx
+++ b/Lab Reports/LabReport10/Lab10SiteData.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abereni4u/Dropbox/Github/PHY121/Lab Reports/LabReport10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522B7034-161E-784A-8A05-CCDEF261B661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAACCB9-B3A6-6549-851C-B2DB6F6BFF76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11200" yWindow="500" windowWidth="12800" windowHeight="14720" xr2:uid="{2B20EF1A-2BA4-C041-9585-172FB9BE588B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14600" activeTab="1" xr2:uid="{2B20EF1A-2BA4-C041-9585-172FB9BE588B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Formatted" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="45">
   <si>
     <t>Initial Mom</t>
   </si>
@@ -74,17 +75,110 @@
     <t>KE Error</t>
   </si>
   <si>
-    <t>ELASTIC COLLISIONS</t>
-  </si>
-  <si>
-    <t>INELASTIC COLLISIONS</t>
+    <t>PART 1: ELASTIC COLLISIONS</t>
+  </si>
+  <si>
+    <t>PART 2: INELASTIC COLLISIONS</t>
+  </si>
+  <si>
+    <t>PART 3: FORCE DURING A COLLISION</t>
+  </si>
+  <si>
+    <t>Initial Velocity</t>
+  </si>
+  <si>
+    <t>Final Velocity</t>
+  </si>
+  <si>
+    <t>Impulse</t>
+  </si>
+  <si>
+    <t>Mass</t>
+  </si>
+  <si>
+    <t>Momentum</t>
+  </si>
+  <si>
+    <t>Percent Difference</t>
+  </si>
+  <si>
+    <t>Trial</t>
+  </si>
+  <si>
+    <t>Impulse (kg m/s)</t>
+  </si>
+  <si>
+    <t>Mass (kg)</t>
+  </si>
+  <si>
+    <t>Percent Difference (\%)</t>
+  </si>
+  <si>
+    <t>tab:part3</t>
+  </si>
+  <si>
+    <t>PART 2: INELASTIC COLLISION</t>
+  </si>
+  <si>
+    <t>Red Cart Mass (kg)</t>
+  </si>
+  <si>
+    <t>Blue Cart Mass (kg)</t>
+  </si>
+  <si>
+    <t>\mathbf{V_f}\textbf{ (m/s)}</t>
+  </si>
+  <si>
+    <t>\mathbf{\Delta{p}}\textbf{ (kg m/s)}</t>
+  </si>
+  <si>
+    <t>\mathbf{V_o}\textbf{ (m/s)}</t>
+  </si>
+  <si>
+    <t>\textbf{Blue Cart }\mathbf{V_o}\textbf{ (m/s)}</t>
+  </si>
+  <si>
+    <t>\textbf{Red Cart }\mathbf{V_o}\textbf{ (m/s)}</t>
+  </si>
+  <si>
+    <t>Total Momentum (kg m/s)</t>
+  </si>
+  <si>
+    <t>Total KE (J)</t>
+  </si>
+  <si>
+    <t>tab:part2pre</t>
+  </si>
+  <si>
+    <t>\textbf{Red Cart }\mathbf{V_f}\textbf{ (m/s)}</t>
+  </si>
+  <si>
+    <t>\textbf{Blue Cart }\mathbf{V_f}\textbf{ (m/s)}</t>
+  </si>
+  <si>
+    <t>Total Momentum \% Difference (%)</t>
+  </si>
+  <si>
+    <t>KE \% Difference (%)</t>
+  </si>
+  <si>
+    <t>tab:part2post</t>
+  </si>
+  <si>
+    <t>PART 1: ELASTIC COLLISION</t>
+  </si>
+  <si>
+    <t>tab:part1pre</t>
+  </si>
+  <si>
+    <t>tab:part1post</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -96,6 +190,26 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
@@ -120,10 +234,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -460,15 +587,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3353EEE6-5D3F-9449-8440-85AAA907E00C}">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView zoomScale="87" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -488,51 +615,57 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
       <c r="E2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" t="s">
-        <v>2</v>
-      </c>
       <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
         <v>3</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>6</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>7</v>
       </c>
-      <c r="M2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
         <v>9</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>10</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -540,205 +673,223 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E3">
-        <f>(A3 *C3) + (B3 *D3)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <f>((1/2)*A3*C3^2)+((1/2)*B3*D3^2)</f>
+        <f>(B3 *D3) + (C3 *E3)</f>
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <f>((1/2)*B3*D3^2)+((1/2)*C3*E3^2)</f>
         <v>12.5</v>
       </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
       <c r="J3">
         <v>1</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M3">
-        <f>(I3 *K3) + (J3 *L3)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N3">
-        <f>((1/2)*I3*K3^2)+((1/2)*J3*L3^2)</f>
+        <v>5</v>
+      </c>
+      <c r="O3">
+        <f>(K3 *M3) + (L3 *N3)</f>
+        <v>5</v>
+      </c>
+      <c r="P3">
+        <f>((1/2)*K3*M3^2)+((1/2)*L3*N3^2)</f>
         <v>12.5</v>
       </c>
-      <c r="O3">
-        <f>ABS((M3-E3)/E3) * 100</f>
-        <v>0</v>
-      </c>
-      <c r="P3" s="1">
-        <f>(ABS((N3-F3)/F3) * 100)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q3">
+        <f>ABS((O3-F3)/F3) * 100</f>
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <f>(ABS((P3-G3)/G3) * 100)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E4">
-        <f>(A4 *C4) + (B4 *D4)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <f>((1/2)*A4*C4^2)+((1/2)*B4*D4^2)</f>
+        <f>(B4 *D4) + (C4 *E4)</f>
+        <v>5</v>
+      </c>
+      <c r="G4">
+        <f>((1/2)*B4*D4^2)+((1/2)*C4*E4^2)</f>
         <v>12.5</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
       <c r="J4">
         <v>2</v>
       </c>
       <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
         <v>-1.7</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>3.3</v>
       </c>
-      <c r="M4">
-        <f>(I4 *K4) + (J4 *L4)</f>
+      <c r="O4">
+        <f>(K4 *M4) + (L4 *N4)</f>
         <v>4.8999999999999995</v>
       </c>
-      <c r="N4">
-        <f>((1/2)*I4*K4^2)+((1/2)*J4*L4^2)</f>
+      <c r="P4">
+        <f>((1/2)*K4*M4^2)+((1/2)*L4*N4^2)</f>
         <v>12.334999999999999</v>
       </c>
-      <c r="O4">
-        <f>ABS((M4-E4)/E4) * 100</f>
+      <c r="Q4">
+        <f>ABS((O4-F4)/F4) * 100</f>
         <v>2.0000000000000107</v>
       </c>
-      <c r="P4" s="1">
-        <f>(ABS((N4-F4)/F4) * 100)</f>
+      <c r="R4">
+        <f>(ABS((P4-G4)/G4) * 100)</f>
         <v>1.3200000000000074</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
         <v>-3</v>
       </c>
-      <c r="E5">
-        <f>(A5 *C5) + (B5 *D5)</f>
-        <v>2</v>
-      </c>
       <c r="F5">
-        <f>((1/2)*A5*C5^2)+((1/2)*B5*D5^2)</f>
+        <f>(B5 *D5) + (C5 *E5)</f>
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <f>((1/2)*B5*D5^2)+((1/2)*C5*E5^2)</f>
         <v>17</v>
       </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
       <c r="J5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
         <v>-3</v>
       </c>
-      <c r="L5">
-        <v>5</v>
-      </c>
-      <c r="M5">
-        <f>(I5 *K5) + (J5 *L5)</f>
-        <v>2</v>
-      </c>
       <c r="N5">
-        <f>((1/2)*I5*K5^2)+((1/2)*J5*L5^2)</f>
+        <v>5</v>
+      </c>
+      <c r="O5">
+        <f>(K5 *M5) + (L5 *N5)</f>
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <f>((1/2)*K5*M5^2)+((1/2)*L5*N5^2)</f>
         <v>17</v>
       </c>
-      <c r="O5">
-        <f>ABS((M5-E5)/E5) * 100</f>
-        <v>0</v>
-      </c>
-      <c r="P5" s="1">
-        <f>(ABS((N5-F5)/F5) * 100)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q5">
+        <f>ABS((O5-F5)/F5) * 100</f>
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <f>(ABS((P5-G5)/G5) * 100)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E6">
-        <f t="shared" ref="E6:E11" si="0">(A6 *C6) + (B6 *D6)</f>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6" si="0">(B6 *D6) + (C6 *E6)</f>
         <v>10</v>
       </c>
-      <c r="F6">
-        <f t="shared" ref="F6:F11" si="1">((1/2)*A6*C6^2)+((1/2)*B6*D6^2)</f>
+      <c r="G6">
+        <f t="shared" ref="G6" si="1">((1/2)*B6*D6^2)+((1/2)*C6*E6^2)</f>
         <v>25</v>
       </c>
-      <c r="I6">
-        <v>2</v>
-      </c>
       <c r="J6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
         <v>1.7</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <v>6.7</v>
       </c>
-      <c r="M6">
-        <f t="shared" ref="M6:M12" si="2">(I6 *K6) + (J6 *L6)</f>
+      <c r="O6">
+        <f t="shared" ref="O6" si="2">(K6 *M6) + (L6 *N6)</f>
         <v>10.1</v>
       </c>
-      <c r="N6">
-        <f t="shared" ref="N6:N12" si="3">((1/2)*I6*K6^2)+((1/2)*J6*L6^2)</f>
+      <c r="P6">
+        <f t="shared" ref="P6" si="3">((1/2)*K6*M6^2)+((1/2)*L6*N6^2)</f>
         <v>25.335000000000001</v>
       </c>
-      <c r="O6">
-        <f t="shared" ref="O6:O12" si="4">ABS((M6-E6)/E6) * 100</f>
+      <c r="Q6">
+        <f>ABS((O6-F6)/F6) * 100</f>
         <v>0.99999999999999634</v>
       </c>
-      <c r="P6" s="1">
-        <f t="shared" ref="P6:P12" si="5">(ABS((N6-F6)/F6) * 100)</f>
+      <c r="R6">
+        <f>(ABS((P6-G6)/G6) * 100)</f>
         <v>1.3400000000000034</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="P7" s="1"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="P8" s="1"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -758,51 +909,57 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
         <v>3</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>4</v>
       </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
       <c r="E10" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
         <v>8</v>
       </c>
-      <c r="I10" t="s">
-        <v>2</v>
-      </c>
       <c r="J10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" t="s">
         <v>3</v>
       </c>
-      <c r="K10" t="s">
+      <c r="M10" t="s">
         <v>6</v>
       </c>
-      <c r="L10" t="s">
+      <c r="N10" t="s">
         <v>7</v>
       </c>
-      <c r="M10" t="s">
-        <v>1</v>
-      </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
+        <v>1</v>
+      </c>
+      <c r="P10" t="s">
         <v>9</v>
       </c>
-      <c r="O10" t="s">
+      <c r="Q10" t="s">
         <v>10</v>
       </c>
-      <c r="P10" t="s">
+      <c r="R10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -810,106 +967,164 @@
         <v>1</v>
       </c>
       <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
         <v>6</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
       <c r="E11">
-        <f>(A11 *C11) + (B11 *D11)</f>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f>(B11 *D11) + (C11 *E11)</f>
         <v>6</v>
       </c>
-      <c r="F11">
-        <f>((1/2)*A11*C11^2)+((1/2)*B11*D11^2)</f>
+      <c r="G11">
+        <f>((1/2)*B11*D11^2)+((1/2)*C11*E11^2)</f>
         <v>18</v>
       </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
       <c r="J11">
         <v>1</v>
       </c>
       <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
         <v>3</v>
       </c>
-      <c r="L11">
+      <c r="N11">
         <v>3</v>
       </c>
-      <c r="M11">
-        <f>(I11 *K11) + (J11 *L11)</f>
+      <c r="O11">
+        <f>(K11 *M11) + (L11 *N11)</f>
         <v>6</v>
       </c>
-      <c r="N11">
-        <f>((1/2)*I11*K11^2)+((1/2)*J11*L11^2)</f>
+      <c r="P11">
+        <f>((1/2)*K11*M11^2)+((1/2)*L11*N11^2)</f>
         <v>9</v>
       </c>
-      <c r="O11">
-        <f>ABS((M11-E11)/E11) * 100</f>
-        <v>0</v>
-      </c>
-      <c r="P11" s="1">
-        <f>(ABS((N11-F11)/F11) * 100)</f>
+      <c r="Q11">
+        <f>ABS((O11-F11)/F11) * 100</f>
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <f>(ABS((P11-G11)/G11) * 100)</f>
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
         <v>3</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>6</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
       <c r="E12">
-        <f t="shared" ref="E12:E14" si="6">(A12 *C12) + (B12 *D12)</f>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ref="F12" si="4">(B12 *D12) + (C12 *E12)</f>
         <v>6</v>
       </c>
-      <c r="F12">
-        <f>((1/2)*A12*C12^2)+((1/2)*B12*D12^2)</f>
+      <c r="G12">
+        <f>((1/2)*B12*D12^2)+((1/2)*C12*E12^2)</f>
         <v>18</v>
       </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
       <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
         <v>3</v>
       </c>
-      <c r="K12">
+      <c r="M12">
         <v>1.5</v>
       </c>
-      <c r="L12">
+      <c r="N12">
         <v>1.5</v>
       </c>
-      <c r="M12">
-        <f>(I12 *K12) + (J12 *L12)</f>
+      <c r="O12">
+        <f>(K12 *M12) + (L12 *N12)</f>
         <v>6</v>
       </c>
-      <c r="N12">
-        <f>((1/2)*I12*K12^2)+((1/2)*J12*L12^2)</f>
+      <c r="P12">
+        <f>((1/2)*K12*M12^2)+((1/2)*L12*N12^2)</f>
         <v>4.5</v>
       </c>
-      <c r="O12">
-        <f>ABS((M12-E12)/E12) * 100</f>
-        <v>0</v>
-      </c>
-      <c r="P12" s="1">
-        <f>(ABS((N12-F12)/F12) * 100)</f>
+      <c r="Q12">
+        <f>ABS((O12-F12)/F12) * 100</f>
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <f>(ABS((P12-G12)/G12) * 100)</f>
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="P13" s="1"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="P14" s="1"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="P15" s="1"/>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>0.65229999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>-0.44090000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>0.31540000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <f>B16*(B18-B17)</f>
+        <v>0.49333448999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>0.47239999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <f>(B19-B20) / (B20) * 100</f>
+        <v>4.4315177815410607</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -918,4 +1133,519 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E31955F-797A-CD45-8534-B5D84878AE6E}">
+  <dimension ref="A2:J26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>0.65229999999999999</v>
+      </c>
+      <c r="B4" s="5">
+        <v>-0.44090000000000001</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.31540000000000001</v>
+      </c>
+      <c r="D4" s="5">
+        <f>A4*(C4-B4)</f>
+        <v>0.49333448999999996</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.47239999999999999</v>
+      </c>
+      <c r="F4" s="5">
+        <f>(D4-E4) / (E4) * 100</f>
+        <v>4.4315177815410607</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>1</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5">
+        <v>6</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <f>(B8 *D8) + (C8 *E8)</f>
+        <v>6</v>
+      </c>
+      <c r="G8" s="5">
+        <f>((1/2)*B8*D8^2)+((1/2)*C8*E8^2)</f>
+        <v>18</v>
+      </c>
+      <c r="H8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>2</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5">
+        <v>3</v>
+      </c>
+      <c r="D9" s="5">
+        <v>6</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <f t="shared" ref="F9" si="0">(B9 *D9) + (C9 *E9)</f>
+        <v>6</v>
+      </c>
+      <c r="G9" s="5">
+        <f>((1/2)*B9*D9^2)+((1/2)*C9*E9^2)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>1</v>
+      </c>
+      <c r="B12" s="7">
+        <v>1</v>
+      </c>
+      <c r="C12" s="7">
+        <v>1</v>
+      </c>
+      <c r="D12" s="7">
+        <v>3</v>
+      </c>
+      <c r="E12" s="7">
+        <v>3</v>
+      </c>
+      <c r="F12" s="7">
+        <v>6</v>
+      </c>
+      <c r="G12" s="7">
+        <v>9</v>
+      </c>
+      <c r="H12" s="7">
+        <v>0</v>
+      </c>
+      <c r="I12" s="7">
+        <v>50</v>
+      </c>
+      <c r="J12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="7">
+        <v>2</v>
+      </c>
+      <c r="B13" s="7">
+        <v>1</v>
+      </c>
+      <c r="C13" s="7">
+        <v>3</v>
+      </c>
+      <c r="D13" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="E13" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="F13" s="7">
+        <v>6</v>
+      </c>
+      <c r="G13" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="H13" s="7">
+        <v>0</v>
+      </c>
+      <c r="I13" s="7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>1</v>
+      </c>
+      <c r="B17" s="5">
+        <v>1</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5">
+        <v>5</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5">
+        <f>(B17 *D17) + (C17 *E17)</f>
+        <v>5</v>
+      </c>
+      <c r="G17" s="5">
+        <f>((1/2)*B17*D17^2)+((1/2)*C17*E17^2)</f>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>2</v>
+      </c>
+      <c r="B18" s="5">
+        <v>1</v>
+      </c>
+      <c r="C18" s="5">
+        <v>2</v>
+      </c>
+      <c r="D18" s="5">
+        <v>5</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0</v>
+      </c>
+      <c r="F18" s="5">
+        <f>(B18 *D18) + (C18 *E18)</f>
+        <v>5</v>
+      </c>
+      <c r="G18" s="5">
+        <f>((1/2)*B18*D18^2)+((1/2)*C18*E18^2)</f>
+        <v>12.5</v>
+      </c>
+      <c r="H18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>3</v>
+      </c>
+      <c r="B19" s="5">
+        <v>1</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1</v>
+      </c>
+      <c r="D19" s="5">
+        <v>5</v>
+      </c>
+      <c r="E19" s="5">
+        <v>-3</v>
+      </c>
+      <c r="F19" s="5">
+        <f>(B19 *D19) + (C19 *E19)</f>
+        <v>2</v>
+      </c>
+      <c r="G19" s="5">
+        <f>((1/2)*B19*D19^2)+((1/2)*C19*E19^2)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>4</v>
+      </c>
+      <c r="B20" s="5">
+        <v>2</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5">
+        <v>5</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0</v>
+      </c>
+      <c r="F20" s="5">
+        <f t="shared" ref="F20" si="1">(B20 *D20) + (C20 *E20)</f>
+        <v>10</v>
+      </c>
+      <c r="G20" s="5">
+        <f t="shared" ref="G20" si="2">((1/2)*B20*D20^2)+((1/2)*C20*E20^2)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>5</v>
+      </c>
+      <c r="F23">
+        <v>5</v>
+      </c>
+      <c r="G23">
+        <v>12.5</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>-1.7</v>
+      </c>
+      <c r="E24">
+        <v>3.3</v>
+      </c>
+      <c r="F24">
+        <v>4.8999999999999995</v>
+      </c>
+      <c r="G24">
+        <v>12.3</v>
+      </c>
+      <c r="H24">
+        <v>2.0000000000000107</v>
+      </c>
+      <c r="I24">
+        <v>1.3200000000000074</v>
+      </c>
+      <c r="J24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>-3</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <v>17</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1.7</v>
+      </c>
+      <c r="E26">
+        <v>6.7</v>
+      </c>
+      <c r="F26">
+        <v>10.1</v>
+      </c>
+      <c r="G26">
+        <v>25.3</v>
+      </c>
+      <c r="H26">
+        <v>0.99999999999999634</v>
+      </c>
+      <c r="I26">
+        <v>1.3400000000000034</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>